<commit_message>
Remove Dockerfile and update .gitignore
The Dockerfile was removed as its hosting setup is no longer required. Additional changes include updating the .gitignore to ignore automatically generated data input files in the config_sheets directory. This is to prevent unnecessary files from being tracked.
</commit_message>
<xml_diff>
--- a/main/data/config_sheets/trnaseq_data_inputs_auto.xlsx
+++ b/main/data/config_sheets/trnaseq_data_inputs_auto.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="naiveB" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="smB" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -559,265 +558,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>FragmentLength</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Layout</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>LibraryPrep</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SampleName</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Strand</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>160.3399623523061</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>smB_S1R1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>164.8370200000294</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>smB_S1R2</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>185.0270003885936</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>smB_S1R3</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>177.2249731723198</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>smB_S1R4</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>single-end</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>smB_S2R1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>single-end</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>smB_S2R2</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>single-end</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>smB_S2R3</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Sort package installation (#140)
</commit_message>
<xml_diff>
--- a/main/data/config_sheets/trnaseq_data_inputs_auto.xlsx
+++ b/main/data/config_sheets/trnaseq_data_inputs_auto.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="naiveB" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="smB" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -559,265 +558,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>FragmentLength</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Layout</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>LibraryPrep</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SampleName</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Strand</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>160.3399623523061</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>smB_S1R1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>164.8370200000294</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>smB_S1R2</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>185.0270003885936</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>smB_S1R3</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>177.2249731723198</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>paired-end</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>smB_S1R4</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>single-end</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>smB_S2R1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>single-end</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>smB_S2R2</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>single-end</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>smB_S2R3</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Include default naiveB and switch memory B cell data
</commit_message>
<xml_diff>
--- a/main/data/config_sheets/trnaseq_data_inputs_auto.xlsx
+++ b/main/data/config_sheets/trnaseq_data_inputs_auto.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="naiveB" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="smB" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -558,4 +559,265 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>FragmentLength</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Group</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Layout</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>LibraryPrep</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>SampleName</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Strand</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>160.3399623523061</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>paired-end</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>smB_S1R1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>164.8370200000294</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>paired-end</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>smB_S1R2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>185.0270003885936</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>paired-end</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>smB_S1R3</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>177.2249731723198</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>paired-end</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>smB_S1R4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>single-end</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>smB_S2R1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>single-end</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>smB_S2R2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>single-end</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>smB_S2R3</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>